<commit_message>
Update workbook and homepage, add slides
</commit_message>
<xml_diff>
--- a/Week-03/Week-03_Workbook.xlsx
+++ b/Week-03/Week-03_Workbook.xlsx
@@ -2,13 +2,8 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mitruong\src\2022-workshop-excel\Week-03\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C218F754-80CB-4C59-97B7-338CE02553E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FE1E9B7-1D5D-4D92-B899-1860E4DD7412}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{AEEA18F0-24A0-46E5-847A-2DF1B3C91941}"/>
   </bookViews>
@@ -38,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="81">
   <si>
     <t>Data</t>
   </si>
@@ -133,9 +128,6 @@
     <t>Age</t>
   </si>
   <si>
-    <t>Comorbidities?</t>
-  </si>
-  <si>
     <t>Registrant001</t>
   </si>
   <si>
@@ -214,20 +206,12 @@
     <t>Thing</t>
   </si>
   <si>
-    <t>Eligible for study?</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
     <t>Yes</t>
   </si>
   <si>
-    <t>Registrants are eligible for this study if:
-- They are under 65 with comorbidities OR
-- They are 65+ with no comorbidities</t>
-  </si>
-  <si>
     <t>Age group</t>
   </si>
   <si>
@@ -240,15 +224,6 @@
     <t>40-64</t>
   </si>
   <si>
-    <t>Group 1</t>
-  </si>
-  <si>
-    <t>Group 2</t>
-  </si>
-  <si>
-    <t>Group 3</t>
-  </si>
-  <si>
     <t>70 and above</t>
   </si>
   <si>
@@ -277,6 +252,32 @@
   </si>
   <si>
     <t>Is it cake?!?</t>
+  </si>
+  <si>
+    <t>Eligibility using OR</t>
+  </si>
+  <si>
+    <t>Comorbidity?</t>
+  </si>
+  <si>
+    <t>BMI</t>
+  </si>
+  <si>
+    <t>Registrants are eligible for this study if they have only one of the following:
+- BMI &gt;30 OR
+- Other comorbidities</t>
+  </si>
+  <si>
+    <t>Eligible using XOR</t>
+  </si>
+  <si>
+    <t>Group A</t>
+  </si>
+  <si>
+    <t>Group B</t>
+  </si>
+  <si>
+    <t>Group C</t>
   </si>
 </sst>
 </file>
@@ -339,7 +340,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -464,11 +465,44 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="2" tint="-9.9948118533890809E-2"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="2" tint="-9.9948118533890809E-2"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="2" tint="-9.9948118533890809E-2"/>
+      </left>
+      <right style="thin">
+        <color theme="2" tint="-9.9948118533890809E-2"/>
+      </right>
+      <top style="thin">
+        <color theme="2" tint="-9.9948118533890809E-2"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2" tint="-9.9948118533890809E-2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -477,13 +511,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -495,6 +539,15 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -504,22 +557,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -963,18 +1003,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F961FAD9-91D9-4E49-B7B0-D958D658468B}">
-  <dimension ref="A1:K25"/>
+  <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.44140625" customWidth="1"/>
-    <col min="3" max="3" width="15.88671875" customWidth="1"/>
-    <col min="4" max="5" width="16.5546875" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="8.21875" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" customWidth="1"/>
+    <col min="6" max="6" width="18.109375" customWidth="1"/>
+    <col min="7" max="7" width="17.88671875" customWidth="1"/>
+    <col min="8" max="8" width="10.77734375" customWidth="1"/>
+    <col min="9" max="9" width="20.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>29</v>
       </c>
@@ -982,353 +1028,506 @@
         <v>30</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" s="2"/>
+      <c r="F1" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>31</v>
-      </c>
-      <c r="D1" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>32</v>
       </c>
       <c r="B2">
         <v>19</v>
       </c>
-      <c r="C2" t="s">
-        <v>59</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="8"/>
-    </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C2">
+        <v>40</v>
+      </c>
+      <c r="D2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" s="7"/>
+      <c r="G2" s="12"/>
+      <c r="I2" s="13"/>
+      <c r="K2" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21"/>
+      <c r="N2" s="21"/>
+      <c r="O2" s="22"/>
+    </row>
+    <row r="3" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3">
         <v>30</v>
       </c>
-      <c r="C3" t="s">
-        <v>60</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="11"/>
-    </row>
-    <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C3">
+        <v>28</v>
+      </c>
+      <c r="D3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3" s="7"/>
+      <c r="G3" s="12"/>
+      <c r="I3" s="13"/>
+      <c r="K3" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
+      <c r="N3" s="18"/>
+      <c r="O3" s="19"/>
+    </row>
+    <row r="4" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B4">
         <v>43</v>
       </c>
-      <c r="C4" t="s">
-        <v>60</v>
-      </c>
-      <c r="G4" s="9"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="11"/>
-    </row>
-    <row r="5" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C4">
+        <v>27</v>
+      </c>
+      <c r="D4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F4" s="7"/>
+      <c r="G4" s="12"/>
+      <c r="I4" s="13"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="18"/>
+      <c r="N4" s="18"/>
+      <c r="O4" s="19"/>
+    </row>
+    <row r="5" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B5">
         <v>77</v>
       </c>
-      <c r="C5" t="s">
-        <v>59</v>
-      </c>
-      <c r="G5" s="9"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="11"/>
-    </row>
-    <row r="6" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C5">
+        <v>27</v>
+      </c>
+      <c r="D5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F5" s="7"/>
+      <c r="G5" s="12"/>
+      <c r="I5" s="13"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="18"/>
+      <c r="N5" s="18"/>
+      <c r="O5" s="19"/>
+    </row>
+    <row r="6" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B6">
         <v>61</v>
       </c>
-      <c r="C6" t="s">
-        <v>59</v>
-      </c>
-      <c r="G6" s="9"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="11"/>
-    </row>
-    <row r="7" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C6">
+        <v>40</v>
+      </c>
+      <c r="D6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F6" s="7"/>
+      <c r="G6" s="12"/>
+      <c r="I6" s="13"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="18"/>
+      <c r="N6" s="18"/>
+      <c r="O6" s="19"/>
+    </row>
+    <row r="7" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B7">
         <v>37</v>
       </c>
-      <c r="C7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C7">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F7" s="7"/>
+      <c r="G7" s="12"/>
+      <c r="I7" s="13"/>
+    </row>
+    <row r="8" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8">
+        <v>27</v>
+      </c>
+      <c r="C8">
+        <v>37</v>
+      </c>
+      <c r="D8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F8" s="7"/>
+      <c r="G8" s="12"/>
+      <c r="I8" s="13"/>
+      <c r="K8" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="L8" s="24"/>
+      <c r="M8" s="24"/>
+      <c r="N8" s="24"/>
+      <c r="O8" s="25"/>
+    </row>
+    <row r="9" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>38</v>
-      </c>
-      <c r="B8">
-        <v>37</v>
-      </c>
-      <c r="C8" t="s">
-        <v>60</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="14"/>
-    </row>
-    <row r="9" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>39</v>
       </c>
       <c r="B9">
         <v>70</v>
       </c>
-      <c r="C9" t="s">
-        <v>59</v>
-      </c>
-      <c r="G9" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="J9" s="15"/>
-      <c r="K9" s="15"/>
-    </row>
-    <row r="10" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C9">
+        <v>39</v>
+      </c>
+      <c r="D9" t="s">
+        <v>57</v>
+      </c>
+      <c r="F9" s="7"/>
+      <c r="G9" s="12"/>
+      <c r="I9" s="13"/>
+      <c r="K9" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="L9" s="16"/>
+      <c r="M9" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="N9" s="16"/>
+      <c r="O9" s="16"/>
+    </row>
+    <row r="10" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B10">
         <v>64</v>
       </c>
-      <c r="C10" t="s">
-        <v>59</v>
-      </c>
-      <c r="G10" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="J10" s="15"/>
-      <c r="K10" s="15"/>
-    </row>
-    <row r="11" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C10">
+        <v>33</v>
+      </c>
+      <c r="D10" t="s">
+        <v>57</v>
+      </c>
+      <c r="F10" s="7"/>
+      <c r="G10" s="12"/>
+      <c r="I10" s="13"/>
+      <c r="K10" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="L10" s="16"/>
+      <c r="M10" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="N10" s="16"/>
+      <c r="O10" s="16"/>
+    </row>
+    <row r="11" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B11">
         <v>44</v>
       </c>
-      <c r="C11" t="s">
-        <v>59</v>
-      </c>
-      <c r="G11" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="J11" s="15"/>
-      <c r="K11" s="15"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C11">
+        <v>40</v>
+      </c>
+      <c r="D11" t="s">
+        <v>57</v>
+      </c>
+      <c r="F11" s="7"/>
+      <c r="G11" s="12"/>
+      <c r="I11" s="13"/>
+      <c r="K11" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="L11" s="16"/>
+      <c r="M11" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="N11" s="16"/>
+      <c r="O11" s="16"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B12">
         <v>80</v>
       </c>
-      <c r="C12" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C12">
+        <v>37</v>
+      </c>
+      <c r="D12" t="s">
+        <v>57</v>
+      </c>
+      <c r="F12" s="7"/>
+      <c r="G12" s="12"/>
+      <c r="I12" s="13"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B13">
         <v>23</v>
       </c>
-      <c r="C13" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C13">
+        <v>37</v>
+      </c>
+      <c r="D13" t="s">
+        <v>58</v>
+      </c>
+      <c r="F13" s="7"/>
+      <c r="G13" s="12"/>
+      <c r="I13" s="13"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B14">
         <v>52</v>
       </c>
-      <c r="C14" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C14">
+        <v>18</v>
+      </c>
+      <c r="D14" t="s">
+        <v>58</v>
+      </c>
+      <c r="F14" s="7"/>
+      <c r="G14" s="12"/>
+      <c r="I14" s="13"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B15">
         <v>69</v>
       </c>
-      <c r="C15" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C15">
+        <v>24</v>
+      </c>
+      <c r="D15" t="s">
+        <v>58</v>
+      </c>
+      <c r="F15" s="7"/>
+      <c r="G15" s="12"/>
+      <c r="I15" s="13"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B16">
         <v>77</v>
       </c>
-      <c r="C16" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C16">
+        <v>38</v>
+      </c>
+      <c r="D16" t="s">
+        <v>58</v>
+      </c>
+      <c r="F16" s="7"/>
+      <c r="G16" s="12"/>
+      <c r="I16" s="13"/>
+      <c r="L16" s="9"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B17">
         <v>50</v>
       </c>
-      <c r="C17" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C17">
+        <v>28</v>
+      </c>
+      <c r="D17" t="s">
+        <v>57</v>
+      </c>
+      <c r="F17" s="7"/>
+      <c r="G17" s="12"/>
+      <c r="I17" s="13"/>
+      <c r="L17" s="9"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B18">
         <v>77</v>
       </c>
-      <c r="C18" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C18">
+        <v>30</v>
+      </c>
+      <c r="D18" t="s">
+        <v>58</v>
+      </c>
+      <c r="F18" s="7"/>
+      <c r="G18" s="12"/>
+      <c r="I18" s="13"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B19">
         <v>73</v>
       </c>
-      <c r="C19" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C19">
+        <v>27</v>
+      </c>
+      <c r="D19" t="s">
+        <v>57</v>
+      </c>
+      <c r="F19" s="7"/>
+      <c r="G19" s="12"/>
+      <c r="I19" s="13"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B20">
         <v>42</v>
       </c>
-      <c r="C20" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C20">
+        <v>21</v>
+      </c>
+      <c r="D20" t="s">
+        <v>57</v>
+      </c>
+      <c r="F20" s="7"/>
+      <c r="G20" s="12"/>
+      <c r="I20" s="13"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B21">
         <v>36</v>
       </c>
-      <c r="C21" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C21">
+        <v>29</v>
+      </c>
+      <c r="D21" t="s">
+        <v>57</v>
+      </c>
+      <c r="F21" s="7"/>
+      <c r="G21" s="12"/>
+      <c r="I21" s="13"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B22">
         <v>59</v>
       </c>
-      <c r="C22" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C22">
+        <v>28</v>
+      </c>
+      <c r="D22" t="s">
+        <v>57</v>
+      </c>
+      <c r="F22" s="7"/>
+      <c r="G22" s="12"/>
+      <c r="I22" s="13"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B23">
         <v>78</v>
       </c>
-      <c r="C23" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C23">
+        <v>21</v>
+      </c>
+      <c r="D23" t="s">
+        <v>57</v>
+      </c>
+      <c r="F23" s="7"/>
+      <c r="G23" s="12"/>
+      <c r="I23" s="13"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B24">
         <v>47</v>
       </c>
-      <c r="C24" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C24">
+        <v>19</v>
+      </c>
+      <c r="D24" t="s">
+        <v>58</v>
+      </c>
+      <c r="F24" s="7"/>
+      <c r="G24" s="12"/>
+      <c r="I24" s="13"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B25">
         <v>69</v>
       </c>
-      <c r="C25" t="s">
-        <v>59</v>
-      </c>
+      <c r="C25">
+        <v>35</v>
+      </c>
+      <c r="D25" t="s">
+        <v>57</v>
+      </c>
+      <c r="F25" s="7"/>
+      <c r="G25" s="12"/>
+      <c r="I25" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="I10:K10"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="G3:K6"/>
-    <mergeCell ref="G2:K2"/>
-    <mergeCell ref="G8:K8"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="M10:O10"/>
+    <mergeCell ref="M11:O11"/>
+    <mergeCell ref="K3:O6"/>
+    <mergeCell ref="K2:O2"/>
+    <mergeCell ref="K8:O8"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="M9:O9"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1351,59 +1550,60 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="22"/>
+        <v>55</v>
+      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="8"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="22"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="8"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="22"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="8"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="22"/>
+        <v>70</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="8"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="22"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="8"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="22"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1427,7 +1627,7 @@
       <c r="B1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="15" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1438,10 +1638,11 @@
       <c r="B2">
         <v>67</v>
       </c>
-      <c r="E2" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="F2" s="16"/>
+      <c r="C2" s="13"/>
+      <c r="E2" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="F2" s="26"/>
     </row>
     <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
@@ -1450,11 +1651,12 @@
       <c r="B3">
         <v>92</v>
       </c>
-      <c r="E3" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="F3" s="17" t="s">
-        <v>70</v>
+      <c r="C3" s="13"/>
+      <c r="E3" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1464,11 +1666,12 @@
       <c r="B4">
         <v>41</v>
       </c>
-      <c r="E4" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="F4" s="17" t="s">
-        <v>72</v>
+      <c r="C4" s="13"/>
+      <c r="E4" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -1478,228 +1681,15 @@
       <c r="B5">
         <v>88</v>
       </c>
+      <c r="C5" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="E2:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100843B1CA7137EAA4AA4D2E2BDF81DB089" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bc1e24afe28d0c357cbe371dee75991f">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5a3927fa-f9bf-4e21-9816-7f925d835449" xmlns:ns3="8424d317-e79a-4f10-a77e-d0bbf29883f4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="295e7143f0b6c41d02b0e37cafda85bc" ns2:_="" ns3:_="">
-    <xsd:import namespace="5a3927fa-f9bf-4e21-9816-7f925d835449"/>
-    <xsd:import namespace="8424d317-e79a-4f10-a77e-d0bbf29883f4"/>
-    <xsd:element name="properties">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element name="documentManagement">
-            <xsd:complexType>
-              <xsd:all>
-                <xsd:element ref="ns2:SharedWithUsers" minOccurs="0"/>
-                <xsd:element ref="ns2:SharedWithDetails" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceMetadata" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceFastMetadata" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceAutoKeyPoints" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceKeyPoints" minOccurs="0"/>
-              </xsd:all>
-            </xsd:complexType>
-          </xsd:element>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="5a3927fa-f9bf-4e21-9816-7f925d835449" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="SharedWithUsers" ma:index="8" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:UserMulti">
-            <xsd:sequence>
-              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
-                <xsd:complexType>
-                  <xsd:sequence>
-                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
-                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
-                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
-                  </xsd:sequence>
-                </xsd:complexType>
-              </xsd:element>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="9" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="8424d317-e79a-4f10-a77e-d0bbf29883f4" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="MediaServiceMetadata" ma:index="10" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceFastMetadata" ma:index="11" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="12" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceKeyPoints" ma:index="13" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
-    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
-    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
-    <xsd:element name="coreProperties" type="CT_coreProperties"/>
-    <xsd:complexType name="CT_coreProperties">
-      <xsd:all>
-        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
-        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
-          <xsd:annotation>
-            <xsd:documentation>
-                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
-                    </xsd:documentation>
-          </xsd:annotation>
-        </xsd:element>
-        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-      </xsd:all>
-    </xsd:complexType>
-  </xsd:schema>
-  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
-    <xs:element name="Person">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:DisplayName" minOccurs="0"/>
-          <xs:element ref="pc:AccountId" minOccurs="0"/>
-          <xs:element ref="pc:AccountType" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="DisplayName" type="xs:string"/>
-    <xs:element name="AccountId" type="xs:string"/>
-    <xs:element name="AccountType" type="xs:string"/>
-    <xs:element name="BDCAssociatedEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-        <xs:attribute ref="pc:EntityNamespace"/>
-        <xs:attribute ref="pc:EntityName"/>
-        <xs:attribute ref="pc:SystemInstanceName"/>
-        <xs:attribute ref="pc:AssociationName"/>
-      </xs:complexType>
-    </xs:element>
-    <xs:attribute name="EntityNamespace" type="xs:string"/>
-    <xs:attribute name="EntityName" type="xs:string"/>
-    <xs:attribute name="SystemInstanceName" type="xs:string"/>
-    <xs:attribute name="AssociationName" type="xs:string"/>
-    <xs:element name="BDCEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
-          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
-          <xs:element ref="pc:EntityId1" minOccurs="0"/>
-          <xs:element ref="pc:EntityId2" minOccurs="0"/>
-          <xs:element ref="pc:EntityId3" minOccurs="0"/>
-          <xs:element ref="pc:EntityId4" minOccurs="0"/>
-          <xs:element ref="pc:EntityId5" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="EntityDisplayName" type="xs:string"/>
-    <xs:element name="EntityInstanceReference" type="xs:string"/>
-    <xs:element name="EntityId1" type="xs:string"/>
-    <xs:element name="EntityId2" type="xs:string"/>
-    <xs:element name="EntityId3" type="xs:string"/>
-    <xs:element name="EntityId4" type="xs:string"/>
-    <xs:element name="EntityId5" type="xs:string"/>
-    <xs:element name="Terms">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermInfo">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermName" minOccurs="0"/>
-          <xs:element ref="pc:TermId" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermName" type="xs:string"/>
-    <xs:element name="TermId" type="xs:string"/>
-  </xs:schema>
-</ct:contentTypeSchema>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3F1E666C-0BB0-40B8-9EDB-8BFAE4A127EC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="5a3927fa-f9bf-4e21-9816-7f925d835449"/>
-    <ds:schemaRef ds:uri="8424d317-e79a-4f10-a77e-d0bbf29883f4"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE016D9D-EC93-4290-A862-831DFBA296F9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
 
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>

<commit_message>
Correct error on Week3 workbook first worksheet
</commit_message>
<xml_diff>
--- a/Week-03/Week-03_Workbook.xlsx
+++ b/Week-03/Week-03_Workbook.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FE1E9B7-1D5D-4D92-B899-1860E4DD7412}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D96C6DB-A05A-4C32-AC5E-5BDB5DFB8B36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{AEEA18F0-24A0-46E5-847A-2DF1B3C91941}"/>
+    <workbookView xWindow="14148" yWindow="2940" windowWidth="7392" windowHeight="7908" xr2:uid="{AEEA18F0-24A0-46E5-847A-2DF1B3C91941}"/>
   </bookViews>
   <sheets>
     <sheet name="Logical Tests" sheetId="6" r:id="rId1"/>
@@ -41,15 +41,6 @@
     <t>Result</t>
   </si>
   <si>
-    <t>B3 is less than 50</t>
-  </si>
-  <si>
-    <t>B2 is greater than 75</t>
-  </si>
-  <si>
-    <t>B4 is equal to 100</t>
-  </si>
-  <si>
     <t>apple</t>
   </si>
   <si>
@@ -62,34 +53,7 @@
     <t>Logical test description</t>
   </si>
   <si>
-    <t>B2 is greater than or equal to B3</t>
-  </si>
-  <si>
-    <t>B3 is less than or equal to B4</t>
-  </si>
-  <si>
-    <t>B4 is not equal to 50 (operator)</t>
-  </si>
-  <si>
-    <t>B2 is not equal to 99 (function)</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>B8 is equal to "apple"</t>
-  </si>
-  <si>
-    <t>B9 is equal to "banana"</t>
-  </si>
-  <si>
-    <t>B10 is equal to "carrot"</t>
-  </si>
-  <si>
-    <t>B11 is greater than 50 and less than 75</t>
-  </si>
-  <si>
-    <t>B12 is greater than 50 or less than 75</t>
   </si>
   <si>
     <t>Status</t>
@@ -278,6 +242,42 @@
   </si>
   <si>
     <t>Group C</t>
+  </si>
+  <si>
+    <t>A2 is greater than 75</t>
+  </si>
+  <si>
+    <t>A3 is less than 50</t>
+  </si>
+  <si>
+    <t>A4 is equal to 100</t>
+  </si>
+  <si>
+    <t>A2 is greater than or equal to A3</t>
+  </si>
+  <si>
+    <t>A3 is less than or equal to A4</t>
+  </si>
+  <si>
+    <t>A4 is not equal to 50 (operator)</t>
+  </si>
+  <si>
+    <t>A8 is equal to "apple"</t>
+  </si>
+  <si>
+    <t>A9 is equal to "banana"</t>
+  </si>
+  <si>
+    <t>A10 is equal to "carrot"</t>
+  </si>
+  <si>
+    <t>A11 is greater than 50 and less than 75</t>
+  </si>
+  <si>
+    <t>A12 is greater than 50 or less than 75</t>
+  </si>
+  <si>
+    <t>A2 is not equal to 99 (function)</t>
   </si>
 </sst>
 </file>
@@ -893,7 +893,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -902,7 +902,7 @@
       </c>
       <c r="B2" s="4"/>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -911,7 +911,7 @@
       </c>
       <c r="B3" s="4"/>
       <c r="C3" t="s">
-        <v>2</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -920,55 +920,55 @@
       </c>
       <c r="B4" s="4"/>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B6" s="4"/>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B7" s="4"/>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -977,7 +977,7 @@
       </c>
       <c r="B11" s="4"/>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -986,13 +986,13 @@
       </c>
       <c r="B12" s="4"/>
       <c r="C12" t="s">
-        <v>18</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B13" s="4"/>
       <c r="C13" t="s">
-        <v>12</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1022,31 +1022,31 @@
   <sheetData>
     <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="10" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="B2">
         <v>19</v>
@@ -1055,13 +1055,13 @@
         <v>40</v>
       </c>
       <c r="D2" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="F2" s="7"/>
       <c r="G2" s="12"/>
       <c r="I2" s="13"/>
       <c r="K2" s="20" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="L2" s="21"/>
       <c r="M2" s="21"/>
@@ -1070,7 +1070,7 @@
     </row>
     <row r="3" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="B3">
         <v>30</v>
@@ -1079,13 +1079,13 @@
         <v>28</v>
       </c>
       <c r="D3" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="F3" s="7"/>
       <c r="G3" s="12"/>
       <c r="I3" s="13"/>
       <c r="K3" s="17" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="L3" s="18"/>
       <c r="M3" s="18"/>
@@ -1094,7 +1094,7 @@
     </row>
     <row r="4" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="B4">
         <v>43</v>
@@ -1103,7 +1103,7 @@
         <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="12"/>
@@ -1116,7 +1116,7 @@
     </row>
     <row r="5" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="B5">
         <v>77</v>
@@ -1125,7 +1125,7 @@
         <v>27</v>
       </c>
       <c r="D5" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="12"/>
@@ -1138,7 +1138,7 @@
     </row>
     <row r="6" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="B6">
         <v>61</v>
@@ -1147,7 +1147,7 @@
         <v>40</v>
       </c>
       <c r="D6" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="12"/>
@@ -1160,7 +1160,7 @@
     </row>
     <row r="7" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="B7">
         <v>37</v>
@@ -1169,7 +1169,7 @@
         <v>21</v>
       </c>
       <c r="D7" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="12"/>
@@ -1177,7 +1177,7 @@
     </row>
     <row r="8" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="B8">
         <v>27</v>
@@ -1186,13 +1186,13 @@
         <v>37</v>
       </c>
       <c r="D8" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="12"/>
       <c r="I8" s="13"/>
       <c r="K8" s="23" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="L8" s="24"/>
       <c r="M8" s="24"/>
@@ -1201,7 +1201,7 @@
     </row>
     <row r="9" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="B9">
         <v>70</v>
@@ -1210,24 +1210,24 @@
         <v>39</v>
       </c>
       <c r="D9" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="12"/>
       <c r="I9" s="13"/>
       <c r="K9" s="16" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="L9" s="16"/>
       <c r="M9" s="16" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="N9" s="16"/>
       <c r="O9" s="16"/>
     </row>
     <row r="10" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="B10">
         <v>64</v>
@@ -1236,24 +1236,24 @@
         <v>33</v>
       </c>
       <c r="D10" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="F10" s="7"/>
       <c r="G10" s="12"/>
       <c r="I10" s="13"/>
       <c r="K10" s="16" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="L10" s="16"/>
       <c r="M10" s="16" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="N10" s="16"/>
       <c r="O10" s="16"/>
     </row>
     <row r="11" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="B11">
         <v>44</v>
@@ -1262,24 +1262,24 @@
         <v>40</v>
       </c>
       <c r="D11" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="F11" s="7"/>
       <c r="G11" s="12"/>
       <c r="I11" s="13"/>
       <c r="K11" s="16" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="L11" s="16"/>
       <c r="M11" s="16" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="N11" s="16"/>
       <c r="O11" s="16"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B12">
         <v>80</v>
@@ -1288,7 +1288,7 @@
         <v>37</v>
       </c>
       <c r="D12" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="F12" s="7"/>
       <c r="G12" s="12"/>
@@ -1296,7 +1296,7 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="B13">
         <v>23</v>
@@ -1305,7 +1305,7 @@
         <v>37</v>
       </c>
       <c r="D13" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="F13" s="7"/>
       <c r="G13" s="12"/>
@@ -1313,7 +1313,7 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="B14">
         <v>52</v>
@@ -1322,7 +1322,7 @@
         <v>18</v>
       </c>
       <c r="D14" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="F14" s="7"/>
       <c r="G14" s="12"/>
@@ -1330,7 +1330,7 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="B15">
         <v>69</v>
@@ -1339,7 +1339,7 @@
         <v>24</v>
       </c>
       <c r="D15" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="F15" s="7"/>
       <c r="G15" s="12"/>
@@ -1347,7 +1347,7 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="B16">
         <v>77</v>
@@ -1356,7 +1356,7 @@
         <v>38</v>
       </c>
       <c r="D16" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="F16" s="7"/>
       <c r="G16" s="12"/>
@@ -1365,7 +1365,7 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="B17">
         <v>50</v>
@@ -1374,7 +1374,7 @@
         <v>28</v>
       </c>
       <c r="D17" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="F17" s="7"/>
       <c r="G17" s="12"/>
@@ -1383,7 +1383,7 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="B18">
         <v>77</v>
@@ -1392,7 +1392,7 @@
         <v>30</v>
       </c>
       <c r="D18" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="12"/>
@@ -1400,7 +1400,7 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="B19">
         <v>73</v>
@@ -1409,7 +1409,7 @@
         <v>27</v>
       </c>
       <c r="D19" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="F19" s="7"/>
       <c r="G19" s="12"/>
@@ -1417,7 +1417,7 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B20">
         <v>42</v>
@@ -1426,7 +1426,7 @@
         <v>21</v>
       </c>
       <c r="D20" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="F20" s="7"/>
       <c r="G20" s="12"/>
@@ -1434,7 +1434,7 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="B21">
         <v>36</v>
@@ -1443,7 +1443,7 @@
         <v>29</v>
       </c>
       <c r="D21" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="F21" s="7"/>
       <c r="G21" s="12"/>
@@ -1451,7 +1451,7 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="B22">
         <v>59</v>
@@ -1460,7 +1460,7 @@
         <v>28</v>
       </c>
       <c r="D22" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="F22" s="7"/>
       <c r="G22" s="12"/>
@@ -1468,7 +1468,7 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="B23">
         <v>78</v>
@@ -1477,7 +1477,7 @@
         <v>21</v>
       </c>
       <c r="D23" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="F23" s="7"/>
       <c r="G23" s="12"/>
@@ -1485,7 +1485,7 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="B24">
         <v>47</v>
@@ -1494,7 +1494,7 @@
         <v>19</v>
       </c>
       <c r="D24" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="F24" s="7"/>
       <c r="G24" s="12"/>
@@ -1502,7 +1502,7 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="B25">
         <v>69</v>
@@ -1511,7 +1511,7 @@
         <v>35</v>
       </c>
       <c r="D25" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="F25" s="7"/>
       <c r="G25" s="12"/>
@@ -1550,53 +1550,53 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="8"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="8"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="8"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="8"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="B6" s="7"/>
       <c r="C6" s="8"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="8"/>
@@ -1611,7 +1611,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4DAC7D8-D06F-46E5-8DAF-411E2FB364AC}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1622,61 +1624,61 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="B2">
         <v>67</v>
       </c>
       <c r="C2" s="13"/>
       <c r="E2" s="26" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="F2" s="26"/>
     </row>
     <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="B3">
         <v>92</v>
       </c>
       <c r="C3" s="13"/>
       <c r="E3" s="6" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="B4">
         <v>41</v>
       </c>
       <c r="C4" s="13"/>
       <c r="E4" s="6" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="B5">
         <v>88</v>

</xml_diff>